<commit_message>
the submit version of the excel for January
</commit_message>
<xml_diff>
--- a/附件1-1【实习生】实习生考勤表-时薪_张宇精.xlsx
+++ b/附件1-1【实习生】实习生考勤表-时薪_张宇精.xlsx
@@ -34,6 +34,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'考勤表-时薪'!$A$2:$Y$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'考勤表-时薪'!$A$2:$Y$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'考勤表-时薪'!$A$2:$Y$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'考勤表-时薪'!$A$2:$Y$42</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -479,11 +480,11 @@
     <numFmt numFmtId="166" formatCode="YYYY\年M\月;@"/>
     <numFmt numFmtId="167" formatCode="0.0\ "/>
     <numFmt numFmtId="168" formatCode="0\ ;[RED]\(0\)"/>
-    <numFmt numFmtId="169" formatCode="&quot;jj&quot;E&quot;wi&quot;SHYY&quot;wi&quot;SHDDDD;@"/>
+    <numFmt numFmtId="169" formatCode="AAAA;@"/>
     <numFmt numFmtId="170" formatCode="0.0\ ;[RED]\(0.0\)"/>
     <numFmt numFmtId="171" formatCode="0.00"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -633,6 +634,13 @@
       <name val="微软雅黑"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <b val="true"/>
@@ -1004,7 +1012,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1080,7 +1088,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1100,31 +1108,31 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="3" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="3" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="25" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="3" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="25" fillId="3" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="3" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="3" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="23" fillId="3" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="24" fillId="3" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1132,7 +1140,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1226,8 +1234,8 @@
   </sheetPr>
   <dimension ref="1:42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z29" activeCellId="0" sqref="Z29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T31" activeCellId="0" sqref="T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="38.25"/>
@@ -1344,7 +1352,7 @@
       <c r="V3" s="14"/>
       <c r="W3" s="15" t="n">
         <f aca="true">TODAY()</f>
-        <v>43140</v>
+        <v>43141</v>
       </c>
       <c r="X3" s="15"/>
       <c r="Y3" s="15"/>
@@ -4447,7 +4455,7 @@
       <c r="V6" s="21"/>
       <c r="W6" s="22" t="n">
         <f aca="false">Y42</f>
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="X6" s="22"/>
       <c r="Y6" s="22"/>
@@ -8558,7 +8566,7 @@
         <v>43121</v>
       </c>
       <c r="B10" s="35" t="n">
-        <v>43093</v>
+        <v>43121</v>
       </c>
       <c r="C10" s="36"/>
       <c r="D10" s="37" t="n">
@@ -9627,7 +9635,7 @@
         <v>43122</v>
       </c>
       <c r="B11" s="35" t="n">
-        <v>43094</v>
+        <v>43122</v>
       </c>
       <c r="C11" s="36"/>
       <c r="D11" s="37" t="n">
@@ -10696,7 +10704,7 @@
         <v>43123</v>
       </c>
       <c r="B12" s="35" t="n">
-        <v>43095</v>
+        <v>43123</v>
       </c>
       <c r="C12" s="36"/>
       <c r="D12" s="37" t="n">
@@ -11765,7 +11773,7 @@
         <v>43124</v>
       </c>
       <c r="B13" s="35" t="n">
-        <v>43096</v>
+        <v>43124</v>
       </c>
       <c r="C13" s="36"/>
       <c r="D13" s="37"/>
@@ -12826,7 +12834,7 @@
         <v>43125</v>
       </c>
       <c r="B14" s="35" t="n">
-        <v>43097</v>
+        <v>43125</v>
       </c>
       <c r="C14" s="36"/>
       <c r="D14" s="37" t="n">
@@ -13895,7 +13903,7 @@
         <v>43126</v>
       </c>
       <c r="B15" s="35" t="n">
-        <v>43098</v>
+        <v>43126</v>
       </c>
       <c r="C15" s="36"/>
       <c r="D15" s="42" t="n">
@@ -14964,7 +14972,7 @@
         <v>43127</v>
       </c>
       <c r="B16" s="35" t="n">
-        <v>43099</v>
+        <v>43127</v>
       </c>
       <c r="C16" s="36"/>
       <c r="D16" s="42"/>
@@ -16025,7 +16033,7 @@
         <v>43128</v>
       </c>
       <c r="B17" s="35" t="n">
-        <v>43100</v>
+        <v>43128</v>
       </c>
       <c r="C17" s="36"/>
       <c r="D17" s="42"/>
@@ -17086,7 +17094,7 @@
         <v>43129</v>
       </c>
       <c r="B18" s="35" t="n">
-        <v>43101</v>
+        <v>43129</v>
       </c>
       <c r="C18" s="36"/>
       <c r="D18" s="45" t="n">
@@ -18155,7 +18163,7 @@
         <v>43130</v>
       </c>
       <c r="B19" s="35" t="n">
-        <v>43102</v>
+        <v>43130</v>
       </c>
       <c r="C19" s="36"/>
       <c r="D19" s="42" t="n">
@@ -19224,7 +19232,7 @@
         <v>43131</v>
       </c>
       <c r="B20" s="35" t="n">
-        <v>43103</v>
+        <v>43131</v>
       </c>
       <c r="C20" s="36"/>
       <c r="D20" s="42" t="n">
@@ -20293,7 +20301,7 @@
         <v>43132</v>
       </c>
       <c r="B21" s="35" t="n">
-        <v>43104</v>
+        <v>43132</v>
       </c>
       <c r="C21" s="36"/>
       <c r="D21" s="45"/>
@@ -21354,7 +21362,7 @@
         <v>43133</v>
       </c>
       <c r="B22" s="35" t="n">
-        <v>43105</v>
+        <v>43133</v>
       </c>
       <c r="C22" s="36"/>
       <c r="D22" s="42" t="n">
@@ -22423,7 +22431,7 @@
         <v>43134</v>
       </c>
       <c r="B23" s="35" t="n">
-        <v>43106</v>
+        <v>43134</v>
       </c>
       <c r="C23" s="36"/>
       <c r="D23" s="45"/>
@@ -23484,7 +23492,7 @@
         <v>43135</v>
       </c>
       <c r="B24" s="35" t="n">
-        <v>43107</v>
+        <v>43135</v>
       </c>
       <c r="C24" s="36"/>
       <c r="D24" s="42"/>
@@ -24537,7 +24545,7 @@
         <v>43136</v>
       </c>
       <c r="B25" s="35" t="n">
-        <v>43108</v>
+        <v>43136</v>
       </c>
       <c r="C25" s="36"/>
       <c r="D25" s="45"/>
@@ -25598,7 +25606,7 @@
         <v>43137</v>
       </c>
       <c r="B26" s="35" t="n">
-        <v>43109</v>
+        <v>43137</v>
       </c>
       <c r="C26" s="36"/>
       <c r="D26" s="42" t="n">
@@ -26667,7 +26675,7 @@
         <v>43138</v>
       </c>
       <c r="B27" s="35" t="n">
-        <v>43110</v>
+        <v>43138</v>
       </c>
       <c r="C27" s="36"/>
       <c r="D27" s="45" t="n">
@@ -27736,7 +27744,7 @@
         <v>43139</v>
       </c>
       <c r="B28" s="35" t="n">
-        <v>43111</v>
+        <v>43139</v>
       </c>
       <c r="C28" s="36"/>
       <c r="D28" s="42"/>
@@ -28797,7 +28805,7 @@
         <v>43140</v>
       </c>
       <c r="B29" s="35" t="n">
-        <v>43112</v>
+        <v>43140</v>
       </c>
       <c r="C29" s="36"/>
       <c r="D29" s="45"/>
@@ -28820,17 +28828,25 @@
       <c r="M29" s="40" t="n">
         <v>30</v>
       </c>
-      <c r="N29" s="39"/>
+      <c r="N29" s="39" t="n">
+        <v>18</v>
+      </c>
       <c r="O29" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="P29" s="40"/>
+      <c r="P29" s="40" t="n">
+        <v>0</v>
+      </c>
       <c r="Q29" s="29"/>
-      <c r="R29" s="37"/>
+      <c r="R29" s="37" t="n">
+        <v>18</v>
+      </c>
       <c r="S29" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="T29" s="40"/>
+      <c r="T29" s="40" t="n">
+        <v>30</v>
+      </c>
       <c r="U29" s="39" t="n">
         <v>23</v>
       </c>
@@ -29850,7 +29866,7 @@
         <v>43141</v>
       </c>
       <c r="B30" s="35" t="n">
-        <v>43113</v>
+        <v>43141</v>
       </c>
       <c r="C30" s="36"/>
       <c r="D30" s="42"/>
@@ -29864,30 +29880,46 @@
       </c>
       <c r="I30" s="40"/>
       <c r="J30" s="29"/>
-      <c r="K30" s="39"/>
+      <c r="K30" s="39" t="n">
+        <v>13</v>
+      </c>
       <c r="L30" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="M30" s="40"/>
-      <c r="N30" s="39"/>
+      <c r="M30" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" s="39" t="n">
+        <v>18</v>
+      </c>
       <c r="O30" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="P30" s="40"/>
+      <c r="P30" s="40" t="n">
+        <v>0</v>
+      </c>
       <c r="Q30" s="29"/>
-      <c r="R30" s="37"/>
+      <c r="R30" s="37" t="n">
+        <v>18</v>
+      </c>
       <c r="S30" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="T30" s="40"/>
-      <c r="U30" s="39"/>
+      <c r="T30" s="40" t="n">
+        <v>30</v>
+      </c>
+      <c r="U30" s="39" t="n">
+        <v>23</v>
+      </c>
       <c r="V30" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="W30" s="40"/>
+      <c r="W30" s="40" t="n">
+        <v>30</v>
+      </c>
       <c r="X30" s="29"/>
       <c r="Y30" s="41" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z30" s="0"/>
       <c r="AA30" s="0"/>
@@ -30895,7 +30927,7 @@
         <v>43142</v>
       </c>
       <c r="B31" s="35" t="n">
-        <v>43114</v>
+        <v>43121</v>
       </c>
       <c r="C31" s="36"/>
       <c r="D31" s="45"/>
@@ -30931,9 +30963,7 @@
       </c>
       <c r="W31" s="40"/>
       <c r="X31" s="29"/>
-      <c r="Y31" s="41" t="n">
-        <v>11</v>
-      </c>
+      <c r="Y31" s="41"/>
       <c r="Z31" s="0"/>
       <c r="AA31" s="0"/>
       <c r="AB31" s="0"/>
@@ -31940,7 +31970,7 @@
         <v>43143</v>
       </c>
       <c r="B32" s="35" t="n">
-        <v>43115</v>
+        <v>43122</v>
       </c>
       <c r="C32" s="36"/>
       <c r="D32" s="42"/>
@@ -32983,7 +33013,7 @@
         <v>43144</v>
       </c>
       <c r="B33" s="35" t="n">
-        <v>43116</v>
+        <v>43123</v>
       </c>
       <c r="C33" s="36"/>
       <c r="D33" s="45"/>
@@ -34026,7 +34056,7 @@
         <v>43145</v>
       </c>
       <c r="B34" s="35" t="n">
-        <v>43117</v>
+        <v>43124</v>
       </c>
       <c r="C34" s="36"/>
       <c r="D34" s="42"/>
@@ -35069,7 +35099,7 @@
         <v>43146</v>
       </c>
       <c r="B35" s="35" t="n">
-        <v>43118</v>
+        <v>43125</v>
       </c>
       <c r="C35" s="36"/>
       <c r="D35" s="45"/>
@@ -36112,7 +36142,7 @@
         <v>43147</v>
       </c>
       <c r="B36" s="35" t="n">
-        <v>43119</v>
+        <v>43126</v>
       </c>
       <c r="C36" s="36"/>
       <c r="D36" s="42"/>
@@ -36120,53 +36150,33 @@
         <v>22</v>
       </c>
       <c r="F36" s="43"/>
-      <c r="G36" s="39" t="n">
-        <v>12</v>
-      </c>
+      <c r="G36" s="39"/>
       <c r="H36" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="I36" s="40" t="n">
-        <v>0</v>
-      </c>
+      <c r="I36" s="40"/>
       <c r="J36" s="29"/>
-      <c r="K36" s="39" t="n">
-        <v>12</v>
-      </c>
+      <c r="K36" s="39"/>
       <c r="L36" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="M36" s="40" t="n">
-        <v>30</v>
-      </c>
-      <c r="N36" s="39" t="n">
-        <v>13</v>
-      </c>
+      <c r="M36" s="40"/>
+      <c r="N36" s="39"/>
       <c r="O36" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="P36" s="40" t="n">
-        <v>30</v>
-      </c>
+      <c r="P36" s="40"/>
       <c r="Q36" s="29"/>
-      <c r="R36" s="37" t="n">
-        <v>17</v>
-      </c>
+      <c r="R36" s="37"/>
       <c r="S36" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="T36" s="40" t="n">
-        <v>0</v>
-      </c>
-      <c r="U36" s="39" t="n">
-        <v>22</v>
-      </c>
+      <c r="T36" s="40"/>
+      <c r="U36" s="39"/>
       <c r="V36" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="W36" s="40" t="n">
-        <v>0</v>
-      </c>
+      <c r="W36" s="40"/>
       <c r="X36" s="29"/>
       <c r="Y36" s="41"/>
       <c r="Z36" s="0"/>
@@ -37175,7 +37185,7 @@
         <v>43148</v>
       </c>
       <c r="B37" s="35" t="n">
-        <v>43120</v>
+        <v>43127</v>
       </c>
       <c r="C37" s="36"/>
       <c r="D37" s="45"/>
@@ -37183,53 +37193,33 @@
         <v>22</v>
       </c>
       <c r="F37" s="46"/>
-      <c r="G37" s="39" t="n">
-        <v>12</v>
-      </c>
+      <c r="G37" s="39"/>
       <c r="H37" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I37" s="40" t="n">
-        <v>0</v>
-      </c>
+      <c r="I37" s="40"/>
       <c r="J37" s="29"/>
-      <c r="K37" s="39" t="n">
-        <v>12</v>
-      </c>
+      <c r="K37" s="39"/>
       <c r="L37" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="M37" s="40" t="n">
-        <v>40</v>
-      </c>
-      <c r="N37" s="39" t="n">
-        <v>18</v>
-      </c>
+      <c r="M37" s="40"/>
+      <c r="N37" s="39"/>
       <c r="O37" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="P37" s="40" t="n">
-        <v>0</v>
-      </c>
+      <c r="P37" s="40"/>
       <c r="Q37" s="29"/>
-      <c r="R37" s="37" t="n">
-        <v>18</v>
-      </c>
+      <c r="R37" s="37"/>
       <c r="S37" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="T37" s="40" t="n">
-        <v>50</v>
-      </c>
-      <c r="U37" s="39" t="n">
-        <v>22</v>
-      </c>
+      <c r="T37" s="40"/>
+      <c r="U37" s="39"/>
       <c r="V37" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="W37" s="40" t="n">
-        <v>0</v>
-      </c>
+      <c r="W37" s="40"/>
       <c r="X37" s="29"/>
       <c r="Y37" s="41"/>
       <c r="Z37" s="0"/>
@@ -38238,7 +38228,7 @@
         <v>43149</v>
       </c>
       <c r="B38" s="35" t="n">
-        <v>43121</v>
+        <v>43128</v>
       </c>
       <c r="C38" s="36"/>
       <c r="D38" s="42"/>
@@ -38246,53 +38236,33 @@
         <v>22</v>
       </c>
       <c r="F38" s="43"/>
-      <c r="G38" s="39" t="n">
-        <v>12</v>
-      </c>
+      <c r="G38" s="39"/>
       <c r="H38" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="I38" s="40" t="n">
-        <v>0</v>
-      </c>
+      <c r="I38" s="40"/>
       <c r="J38" s="29"/>
-      <c r="K38" s="39" t="n">
-        <v>12</v>
-      </c>
+      <c r="K38" s="39"/>
       <c r="L38" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="M38" s="40" t="n">
-        <v>40</v>
-      </c>
-      <c r="N38" s="39" t="n">
-        <v>18</v>
-      </c>
+      <c r="M38" s="40"/>
+      <c r="N38" s="39"/>
       <c r="O38" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="P38" s="40" t="n">
-        <v>0</v>
-      </c>
+      <c r="P38" s="40"/>
       <c r="Q38" s="29"/>
-      <c r="R38" s="37" t="n">
-        <v>18</v>
-      </c>
+      <c r="R38" s="37"/>
       <c r="S38" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="T38" s="40" t="n">
-        <v>50</v>
-      </c>
-      <c r="U38" s="39" t="n">
-        <v>22</v>
-      </c>
+      <c r="T38" s="40"/>
+      <c r="U38" s="39"/>
       <c r="V38" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="W38" s="40" t="n">
-        <v>30</v>
-      </c>
+      <c r="W38" s="40"/>
       <c r="X38" s="29"/>
       <c r="Y38" s="41"/>
       <c r="Z38" s="0"/>
@@ -39301,7 +39271,7 @@
         <v>43150</v>
       </c>
       <c r="B39" s="35" t="n">
-        <v>43122</v>
+        <v>43129</v>
       </c>
       <c r="C39" s="36"/>
       <c r="D39" s="48"/>
@@ -39309,53 +39279,33 @@
         <v>22</v>
       </c>
       <c r="F39" s="49"/>
-      <c r="G39" s="39" t="n">
-        <v>12</v>
-      </c>
+      <c r="G39" s="39"/>
       <c r="H39" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="I39" s="40" t="n">
-        <v>0</v>
-      </c>
+      <c r="I39" s="40"/>
       <c r="J39" s="29"/>
-      <c r="K39" s="39" t="n">
-        <v>12</v>
-      </c>
+      <c r="K39" s="39"/>
       <c r="L39" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="M39" s="40" t="n">
-        <v>40</v>
-      </c>
-      <c r="N39" s="39" t="n">
-        <v>18</v>
-      </c>
+      <c r="M39" s="40"/>
+      <c r="N39" s="39"/>
       <c r="O39" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="P39" s="40" t="n">
-        <v>0</v>
-      </c>
+      <c r="P39" s="40"/>
       <c r="Q39" s="29"/>
-      <c r="R39" s="37" t="n">
-        <v>18</v>
-      </c>
+      <c r="R39" s="37"/>
       <c r="S39" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="T39" s="40" t="n">
-        <v>50</v>
-      </c>
-      <c r="U39" s="39" t="n">
-        <v>23</v>
-      </c>
+      <c r="T39" s="40"/>
+      <c r="U39" s="39"/>
       <c r="V39" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="W39" s="40" t="n">
-        <v>0</v>
-      </c>
+      <c r="W39" s="40"/>
       <c r="X39" s="29"/>
       <c r="Y39" s="41"/>
       <c r="Z39" s="0"/>
@@ -40364,7 +40314,7 @@
         <v>43151</v>
       </c>
       <c r="B40" s="35" t="n">
-        <v>43123</v>
+        <v>43130</v>
       </c>
       <c r="C40" s="36"/>
       <c r="D40" s="48"/>
@@ -40372,34 +40322,22 @@
         <v>22</v>
       </c>
       <c r="F40" s="49"/>
-      <c r="G40" s="39" t="n">
-        <v>12</v>
-      </c>
+      <c r="G40" s="39"/>
       <c r="H40" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I40" s="40" t="n">
-        <v>0</v>
-      </c>
+      <c r="I40" s="40"/>
       <c r="J40" s="29"/>
-      <c r="K40" s="39" t="n">
-        <v>12</v>
-      </c>
+      <c r="K40" s="39"/>
       <c r="L40" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="M40" s="40" t="n">
-        <v>30</v>
-      </c>
-      <c r="N40" s="39" t="n">
-        <v>15</v>
-      </c>
+      <c r="M40" s="40"/>
+      <c r="N40" s="39"/>
       <c r="O40" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="P40" s="40" t="n">
-        <v>30</v>
-      </c>
+      <c r="P40" s="40"/>
       <c r="Q40" s="29"/>
       <c r="R40" s="37"/>
       <c r="S40" s="51" t="s">
@@ -40470,7 +40408,7 @@
       <c r="X42" s="63"/>
       <c r="Y42" s="65" t="n">
         <f aca="false">SUM(Y10:Y40)</f>
-        <v>235</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>